<commit_message>
calculate unloaded aircraft moments of inertia (minus fuselage stuff)
</commit_message>
<xml_diff>
--- a/physics/propulsion/Propulsion System Configs/IMPORT/6S Battery Data Condensed.xlsx
+++ b/physics/propulsion/Propulsion System Configs/IMPORT/6S Battery Data Condensed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamt\OneDrive\Organized\Engineering\Academics\NCSU\Fall 2025\MAE 480 Aerospace Vehicle Design\MDAO\physics\propulsion\Propulsion System Configs\IMPORT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F69EE2-5FE4-491A-9DA4-13551B37F5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616BF445-3073-4ABB-B6FE-F01B8BA4FF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Battery Name</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>https://www.amazon.com/TATTU-4500mAh-22-2V-6S1P-Battery/dp/B0CDH68NQC/ref=sr_1_17?crid=2MVIQ8OZE2WUW&amp;dib=eyJ2IjoiMSJ9.IKq6sjdeLyWWJxsCIiAP1RCM5LKmsTmkUITrzqPX2BuRL8l3Rdv7_bdeaEa2D1vRWSdY8d3OMi1E7BFt-CBYHvUDstOCb6HTvuA4dT84Gsm-y1r1Gqh1Nas_hPlGq8mkr5HmN8Mj63jqDI7HXwxD2k2AmyOEgb4faMbznZVO0lhFfH2XEBFO2gVRN223MxLkzRFH3ZN0wFPa9wiRv7pC41NflGrQ1stdpVrQXDG0Vay7ow08gVkDvK0pOOt9RgPbEx_WoO6zHJ9MgiFgO0l1UQXZj_nvGtEKStVCCeMr6uQ.ynVftL2T531sEYjp1eAweE0ktp3Cj06ydrgKzLxQUek&amp;dib_tag=se&amp;keywords=22.2+V+4500+mAh&amp;qid=1758825577&amp;sprefix=22.2+v+4500+mah%2Caps%2C137&amp;sr=8-17</t>
+  </si>
+  <si>
+    <t>Length (in)</t>
+  </si>
+  <si>
+    <t>Width (in)</t>
+  </si>
+  <si>
+    <t>Height (in)</t>
   </si>
 </sst>
 </file>
@@ -146,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -169,11 +178,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -185,6 +205,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,10 +426,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -416,7 +439,7 @@
     <col min="6" max="6" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,8 +467,17 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -476,8 +508,17 @@
       <c r="I2" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="J2">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="K2">
+        <v>1.36</v>
+      </c>
+      <c r="L2">
+        <v>1.91</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -508,8 +549,17 @@
       <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="J3">
+        <v>5.44</v>
+      </c>
+      <c r="K3">
+        <v>1.69</v>
+      </c>
+      <c r="L3">
+        <v>1.64</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -540,8 +590,17 @@
       <c r="I4" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="J4">
+        <v>5.46</v>
+      </c>
+      <c r="K4">
+        <v>1.69</v>
+      </c>
+      <c r="L4">
+        <v>1.99</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -572,18 +631,27 @@
       <c r="I5" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="J5">
+        <v>5.43</v>
+      </c>
+      <c r="K5">
+        <v>1.65</v>
+      </c>
+      <c r="L5">
+        <v>2.04</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>